<commit_message>
Fixed CAN wrapper and 1st test
</commit_message>
<xml_diff>
--- a/Config/Documents/VPC_2530b_7_22.xlsx
+++ b/Config/Documents/VPC_2530b_7_22.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\GIP-FCT\Config\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{606FA91D-58F0-4A49-87C0-8AFACB6525EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{115F3184-9F2B-483A-BD72-DF47723FBE0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13992" activeTab="3" xr2:uid="{C3A94F00-46C4-4B6F-8109-6284738D3D4E}"/>
+    <workbookView xWindow="1404" yWindow="1914" windowWidth="17280" windowHeight="12798" activeTab="3" xr2:uid="{C3A94F00-46C4-4B6F-8109-6284738D3D4E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1617,7 +1617,7 @@
     <t>GP1_VB_COMBINED</t>
   </si>
   <si>
-    <t>TP</t>
+    <t>GP1_GRID_1A_OUT</t>
   </si>
 </sst>
 </file>
@@ -11605,8 +11605,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BFAEE26-8A5C-4F36-9E9A-EBBBCEFA4134}">
   <dimension ref="A2:S74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F45" sqref="F45"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F34" sqref="F20:F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>

</xml_diff>